<commit_message>
in progress. Fixed invalid csv deposit date
</commit_message>
<xml_diff>
--- a/test/testdata/testSBEarningUsdc_uniqueOwner_1_deposit_1_partial_withdr.xlsx
+++ b/test/testdata/testSBEarningUsdc_uniqueOwner_1_deposit_1_partial_withdr.xlsx
@@ -327,12 +327,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#0.##"/>
     <numFmt numFmtId="165" formatCode="#0.#######"/>
     <numFmt numFmtId="166" formatCode="#0.###"/>
     <numFmt numFmtId="167" formatCode="#0.########"/>
     <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -477,10 +478,10 @@
     <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,7 +808,9 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="29.07421875" customWidth="1"/>
-    <col min="3" max="10" width="14.921875" customWidth="1"/>
+    <col min="3" max="8" width="14.921875" customWidth="1"/>
+    <col min="9" max="9" width="18.84375" customWidth="1"/>
+    <col min="10" max="10" width="14.921875" customWidth="1"/>
     <col min="11" max="11" width="69.921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -852,19 +855,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="26.15" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
@@ -2043,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="5">
-        <v>9.62381829188962</v>
+        <v>11.111261485697399</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="4" t="s">
@@ -2072,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="5">
-        <v>7.9457452801725603</v>
+        <v>8.6074164041601797</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="4" t="s">
@@ -2101,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="5">
-        <v>9.9581720247588201</v>
+        <v>9.2405371407476196</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="4" t="s">
@@ -2130,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="5">
-        <v>4.6773708951095596</v>
+        <v>5.5965333255953702</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="4" t="s">
@@ -2159,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="5">
-        <v>6.02568500304187</v>
+        <v>5.2242878128563497</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="4" t="s">
@@ -2167,9 +2170,9 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="I47" s="11">
+      <c r="I47" s="12">
         <f>SUM(I42:I46)</f>
-        <v>38.230791494972429</v>
+        <v>39.780036169056913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>